<commit_message>
modifiche minori testo visibile e aggiornato glossario
</commit_message>
<xml_diff>
--- a/data/glossary.xlsx
+++ b/data/glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcolonghin/Desktop/POM Unimore/Database PCM_Hub/progetto_lingue_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0727B49D-CF55-5247-BD2C-C0E7E13973BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F9E08-E430-6A47-87D6-AD73F91EDAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="DatiEsterni_3" localSheetId="3" hidden="1">motivations!$A$1:$B$5</definedName>
     <definedName name="DatiEsterni_4" localSheetId="2" hidden="1">languages!$A$1:$I$4</definedName>
     <definedName name="DatiEsterni_5" localSheetId="1" hidden="1">language_parameters!$A$1:$D$2</definedName>
-    <definedName name="DatiEsterni_6" localSheetId="0" hidden="1">glossary!$A$1:$B$23</definedName>
+    <definedName name="DatiEsterni_6" localSheetId="0" hidden="1">glossary!$A$1:$B$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -314,9 +314,6 @@
     <t>How to distinguish case suffixes from postpositions in postpositional languages: \n1. the case suffix occurs on a head noun or adjective before some other phrase-internal word (another adjective, a relative clause…), OR \n2. the case suffix occurs both on the head noun, and some other phrase-internal category (adjective, quantifier, demonstrative) agrees with it through a corresponding suffix, OR \n3. the case suffix is only on the head noun but it is more internal than other noun suffixes, such as e.g. of Number, possessed status, etc.</t>
   </si>
   <si>
-    <t>It is used to refer to a determiner that does not express any meaning other than (in)definiteness or just φ-features, and sometimes even less interpretable content (expletive articles). In some languages, articles (normally phonologically unstressed) occur as morphosyntactically free morphemes, in others they are bound morphemes affixed to the head noun (or an adjective).</t>
-  </si>
-  <si>
     <t>The interpretation of the denotatum of a nominal phrase as being considered maximal in the shared domain of discourse, in many languages provided by designated articles, by demonstratives, possessives, or inherited even at a distance from certain Genitives. Definite arguments can be specific (i.e. assume the existence of a denotatum) or non-specific, and definiteness and specificity must by no means be confused.</t>
   </si>
   <si>
@@ -375,6 +372,23 @@
   </si>
   <si>
     <t>INSERIRE DESCRIZIONE</t>
+  </si>
+  <si>
+    <t>It is used to refer to a determiner that does not express any meaning other than (in)definiteness or just phi-features, and sometimes even less interpretable content (expletive articles). In some languages, articles (normally phonologically unstressed) occur as morphosyntactically free morphemes, in others they are bound morphemes affixed to the head noun (or an adjective).</t>
+  </si>
+  <si>
+    <t>Atomizing</t>
+  </si>
+  <si>
+    <t>The process shifting the interpretation of a nominal argument from an unbounded reading (a free variable, indirectly bound) to a bounded one (a variable bound by a specific determiner).</t>
+  </si>
+  <si>
+    <t>(morphological) Case</t>
+  </si>
+  <si>
+    <t>In nominal morphology it is important to have a demarcation criterion between inflectional (lato sensu, i.e. including agglutinative morphology) Case proper and pre-/post-positional words. Two criteria are conceivable, as a first approximation:
+a. many prepositional languages have Case suffixes, so that they are easily distinguished positionally from phrase-initial functional words like prepositions
+b. for postpositional languages, a demarcation criterion between Case-suffixes and postpositions is necessary, however. A distinction can be made if: 1) the suffix occurs on a head noun or adjective before some other phrase-internal word (another adjective, a relative clause...) or 2) the suffix occurs both on the head noun and some other phrase-internal category (adjective, quantifier, demonstrative) agrees with it through a corresponding suffix  or 3) the suffix is only on the head noun but, in the morphological structure, it is more word-internal than other noun suffixes, such as eg. of number, possessed status etc.</t>
   </si>
 </sst>
 </file>
@@ -416,17 +430,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -599,11 +639,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F340FC1D-A39C-497B-A12A-203D6EEE8939}" name="glossary" displayName="glossary" ref="A1:B23" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B23" xr:uid="{F340FC1D-A39C-497B-A12A-203D6EEE8939}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F340FC1D-A39C-497B-A12A-203D6EEE8939}" name="glossary" displayName="glossary" ref="A1:B25" tableType="queryTable" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B25" xr:uid="{F340FC1D-A39C-497B-A12A-203D6EEE8939}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6AD0E5FA-E6E1-4977-8554-0E3F5A8A2846}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{AD70B954-308E-4AE6-9F7C-C58B10D620F3}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{6AD0E5FA-E6E1-4977-8554-0E3F5A8A2846}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{AD70B954-308E-4AE6-9F7C-C58B10D620F3}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -613,10 +653,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2F1D94D5-DF83-412F-95D7-257D789455D6}" name="language_parameters" displayName="language_parameters" ref="A1:D2" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{2F1D94D5-DF83-412F-95D7-257D789455D6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{14A2F1A0-D2BC-413C-A1BF-9CDDE9BAFD3C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{66FB62D3-0D35-4E42-A49A-2ED327F03CDF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{2E7860B0-19F5-4032-828D-DACA884636A2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{1023FE2E-CC19-4106-852B-5222DF2A5CB2}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{14A2F1A0-D2BC-413C-A1BF-9CDDE9BAFD3C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{66FB62D3-0D35-4E42-A49A-2ED327F03CDF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{2E7860B0-19F5-4032-828D-DACA884636A2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1023FE2E-CC19-4106-852B-5222DF2A5CB2}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,15 +666,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F6F074D7-90B2-4EBA-B27B-29F5B9880FD4}" name="languages" displayName="languages" ref="A1:I4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I4" xr:uid="{F6F074D7-90B2-4EBA-B27B-29F5B9880FD4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{85D3913A-4C11-4A90-8B64-A1E899E80067}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{CF6E9D61-2619-43FB-9CD7-73D9B4D0C4AE}" uniqueName="2" name="name_full" queryTableFieldId="2" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{85D3913A-4C11-4A90-8B64-A1E899E80067}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{CF6E9D61-2619-43FB-9CD7-73D9B4D0C4AE}" uniqueName="2" name="name_full" queryTableFieldId="2" dataDxfId="22"/>
     <tableColumn id="3" xr3:uid="{4EF19EA2-9C2D-4DBC-9616-F0F90B70DEBC}" uniqueName="3" name="position" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{569493CA-2A58-44E9-B82E-C184B545F7F9}" uniqueName="4" name="grp" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{9CAEA168-496C-497C-8268-94C2C148C888}" uniqueName="5" name="isocode" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{5EE5FAA6-3FFC-48F1-A8A5-C3EAC80F1A2E}" uniqueName="6" name="glottocode" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{6267B2BF-D48B-4694-82A9-AE9B2EA9F8E7}" uniqueName="7" name="informant" queryTableFieldId="7" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{D83AA30F-ECB3-498A-BCB5-48554E351CAD}" uniqueName="8" name="supervisor" queryTableFieldId="8" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{AE8AA8EE-0214-4139-B2AB-E1D7510F9A18}" uniqueName="9" name="assigned_user_email" queryTableFieldId="9" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{569493CA-2A58-44E9-B82E-C184B545F7F9}" uniqueName="4" name="grp" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{9CAEA168-496C-497C-8268-94C2C148C888}" uniqueName="5" name="isocode" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{5EE5FAA6-3FFC-48F1-A8A5-C3EAC80F1A2E}" uniqueName="6" name="glottocode" queryTableFieldId="6" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{6267B2BF-D48B-4694-82A9-AE9B2EA9F8E7}" uniqueName="7" name="informant" queryTableFieldId="7" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{D83AA30F-ECB3-498A-BCB5-48554E351CAD}" uniqueName="8" name="supervisor" queryTableFieldId="8" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{AE8AA8EE-0214-4139-B2AB-E1D7510F9A18}" uniqueName="9" name="assigned_user_email" queryTableFieldId="9" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -644,8 +684,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AEDD5ED6-C713-4EDC-A06B-4DD57BF4AB1F}" name="motivations" displayName="motivations" ref="A1:B5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B5" xr:uid="{AEDD5ED6-C713-4EDC-A06B-4DD57BF4AB1F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8CCA0FA6-DA67-418E-8B26-C9962310971F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{68C3EA7A-1D4F-4E74-8007-BD245D61523E}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{8CCA0FA6-DA67-418E-8B26-C9962310971F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{68C3EA7A-1D4F-4E74-8007-BD245D61523E}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -655,12 +695,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C7C4FF96-1B6D-4CCA-9D5E-67C67057AEDF}" name="parameters" displayName="parameters" ref="A1:G4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G4" xr:uid="{C7C4FF96-1B6D-4CCA-9D5E-67C67057AEDF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0B6068A2-9922-466D-B9D5-A33D985D3336}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{1F6245EA-C647-4228-9207-2B729F2F0CB5}" uniqueName="2" name="name" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{9424F12B-EAF0-4846-A8B1-CA748E224ED5}" uniqueName="3" name="short_description" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{0B6068A2-9922-466D-B9D5-A33D985D3336}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1F6245EA-C647-4228-9207-2B729F2F0CB5}" uniqueName="2" name="name" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{9424F12B-EAF0-4846-A8B1-CA748E224ED5}" uniqueName="3" name="short_description" queryTableFieldId="3" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{943E732B-797E-4A4E-AE88-4AC36D5AA185}" uniqueName="4" name="position" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C3AD8CCC-CD6B-4003-A8E2-AA344034E95B}" uniqueName="5" name="is_active" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{38B6776C-7702-42B7-B827-0C9448614A2E}" uniqueName="6" name="implicational_condition" queryTableFieldId="6" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{38B6776C-7702-42B7-B827-0C9448614A2E}" uniqueName="6" name="implicational_condition" queryTableFieldId="6" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{CFC3CDD1-EF4F-4F41-869A-AD1039F6927F}" uniqueName="7" name="warning_default" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -671,12 +711,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E6C3B46-30C3-4A7B-AB14-3BC2994EBC03}" name="questions" displayName="questions" ref="A1:G5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G5" xr:uid="{9E6C3B46-30C3-4A7B-AB14-3BC2994EBC03}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{67101A1B-8988-4C10-B195-721AF4A4DDFE}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DAC026A4-4E08-45C5-B847-62B6EE459D89}" uniqueName="2" name="parameter_id" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D9BAD92C-B225-46BB-B2D0-72E22D71473D}" uniqueName="3" name="text" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2D445D34-3D4E-46E5-A031-AEF21A353ACC}" uniqueName="4" name="example_yes" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1A723189-B285-4202-A439-2A700C433930}" uniqueName="5" name="instruction" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{346B1415-F909-425C-8E39-5140B8FB4AE1}" uniqueName="6" name="template_type" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{67101A1B-8988-4C10-B195-721AF4A4DDFE}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{DAC026A4-4E08-45C5-B847-62B6EE459D89}" uniqueName="2" name="parameter_id" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{D9BAD92C-B225-46BB-B2D0-72E22D71473D}" uniqueName="3" name="text" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{2D445D34-3D4E-46E5-A031-AEF21A353ACC}" uniqueName="4" name="example_yes" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{1A723189-B285-4202-A439-2A700C433930}" uniqueName="5" name="instruction" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{346B1415-F909-425C-8E39-5140B8FB4AE1}" uniqueName="6" name="template_type" queryTableFieldId="6" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{364735F5-D972-427D-BA27-3715C335102D}" uniqueName="7" name="is_stop_question" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -946,200 +986,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A27F97-E596-4BB0-99B8-D16553F1AC72}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="127.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" ht="43" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:2" ht="43" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:2" ht="43" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>103</v>
+    </row>
+    <row r="24" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="112" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>